<commit_message>
Added Endorsment and updated test data
</commit_message>
<xml_diff>
--- a/CucumberTest/src/TestData/TestData.xlsx
+++ b/CucumberTest/src/TestData/TestData.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NastasjaDamjanac\Desktop\SmokeSandbox\Sandbox-Automation-Smoke-Test\CucumberTest\src\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adragutinovic\Desktop\Projekti\Sandbox Smoke\Sandbox-Automation-Smoke-Test\CucumberTest\src\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69899328-D7E5-4670-9E5D-E2F882D8BA23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F9FA1CA-4EF6-4A30-A120-7338F0CECFA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{D341BFEF-FEF1-4343-8272-FBF06FB03C18}"/>
+    <workbookView xWindow="528" yWindow="468" windowWidth="21504" windowHeight="11256" activeTab="3" xr2:uid="{D341BFEF-FEF1-4343-8272-FBF06FB03C18}"/>
   </bookViews>
   <sheets>
     <sheet name="PersonalAutoData" sheetId="1" r:id="rId1"/>
     <sheet name="CustomerData" sheetId="4" r:id="rId2"/>
     <sheet name="VehicleData" sheetId="6" r:id="rId3"/>
+    <sheet name="EndorsementData" sheetId="7" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="72">
   <si>
     <t>Program</t>
   </si>
@@ -233,6 +234,27 @@
   </si>
   <si>
     <t>4-Door Sedan | 2WD | 5.0 Ltrs | 4x2</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Reason</t>
+  </si>
+  <si>
+    <t>Sub_Type</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Endorsement</t>
+  </si>
+  <si>
+    <t>Policy Correction</t>
+  </si>
+  <si>
+    <t>Add Vehicle</t>
   </si>
 </sst>
 </file>
@@ -660,7 +682,7 @@
   <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I1" sqref="I1"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -911,8 +933,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E138985-DD5C-455A-A3EE-C1D37B547FBC}">
   <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L11" sqref="L11"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -996,4 +1018,65 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19DA6AE0-FD1B-43DF-B1FC-EADB519F14FB}">
+  <dimension ref="A1:E3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="15.6640625" customWidth="1"/>
+    <col min="2" max="2" width="20" customWidth="1"/>
+    <col min="3" max="3" width="27.5546875" customWidth="1"/>
+    <col min="4" max="4" width="18.109375" customWidth="1"/>
+    <col min="5" max="5" width="18.88671875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" s="3"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added Cancellation and Reinstatement. Updated Test Data
</commit_message>
<xml_diff>
--- a/CucumberTest/src/TestData/TestData.xlsx
+++ b/CucumberTest/src/TestData/TestData.xlsx
@@ -8,15 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adragutinovic\Desktop\Projekti\Sandbox Smoke\Sandbox-Automation-Smoke-Test\CucumberTest\src\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F9FA1CA-4EF6-4A30-A120-7338F0CECFA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9ECD829A-3F23-4511-A75A-9FFB994B058D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="528" yWindow="468" windowWidth="21504" windowHeight="11256" activeTab="3" xr2:uid="{D341BFEF-FEF1-4343-8272-FBF06FB03C18}"/>
+    <workbookView xWindow="528" yWindow="468" windowWidth="21504" windowHeight="11256" firstSheet="1" activeTab="5" xr2:uid="{D341BFEF-FEF1-4343-8272-FBF06FB03C18}"/>
   </bookViews>
   <sheets>
     <sheet name="PersonalAutoData" sheetId="1" r:id="rId1"/>
     <sheet name="CustomerData" sheetId="4" r:id="rId2"/>
     <sheet name="VehicleData" sheetId="6" r:id="rId3"/>
     <sheet name="EndorsementData" sheetId="7" r:id="rId4"/>
+    <sheet name="CancelationData" sheetId="8" r:id="rId5"/>
+    <sheet name="ReinstatementData" sheetId="9" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -39,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="80">
   <si>
     <t>Program</t>
   </si>
@@ -255,13 +257,37 @@
   </si>
   <si>
     <t>Add Vehicle</t>
+  </si>
+  <si>
+    <t>Method</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cancellation Insured </t>
+  </si>
+  <si>
+    <t>Cancellation</t>
+  </si>
+  <si>
+    <t>Other</t>
+  </si>
+  <si>
+    <t>Pro Rate</t>
+  </si>
+  <si>
+    <t>Claims</t>
+  </si>
+  <si>
+    <t>Reinstatement</t>
+  </si>
+  <si>
+    <t>Premium Paid</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -297,8 +323,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF222222"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -323,8 +356,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -347,12 +386,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -364,6 +412,8 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1024,8 +1074,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19DA6AE0-FD1B-43DF-B1FC-EADB519F14FB}">
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1038,19 +1088,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="12" t="s">
         <v>68</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="12" t="s">
         <v>67</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="12" t="s">
         <v>66</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="12" t="s">
         <v>55</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="E1" s="12" t="s">
         <v>65</v>
       </c>
     </row>
@@ -1079,4 +1129,111 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D49D3F3-CDFD-45AB-BBBE-4F6B62388EC6}">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:E1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="18.33203125" customWidth="1"/>
+    <col min="2" max="2" width="13.33203125" customWidth="1"/>
+    <col min="3" max="3" width="11.33203125" customWidth="1"/>
+    <col min="4" max="4" width="8.77734375" customWidth="1"/>
+    <col min="5" max="5" width="10.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="D1" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="E1" s="12" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5EB7EE2A-FBF3-479E-892C-1E311A47FC74}">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="14" customWidth="1"/>
+    <col min="2" max="2" width="15.5546875" customWidth="1"/>
+    <col min="3" max="3" width="12.5546875" customWidth="1"/>
+    <col min="5" max="5" width="14.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="D1" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="E1" s="12" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Fixed NB steps and added steps for diary and cancellation
</commit_message>
<xml_diff>
--- a/CucumberTest/src/TestData/TestData.xlsx
+++ b/CucumberTest/src/TestData/TestData.xlsx
@@ -8,17 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NastasjaDamjanac\Desktop\SmokeSandbox\Sandbox-Automation-Smoke-Test\CucumberTest\src\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE734237-646F-4BD1-9614-E8A1EF200D04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F325126D-7237-44F8-B184-029DA25F4740}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="1" activeTab="4" xr2:uid="{D341BFEF-FEF1-4343-8272-FBF06FB03C18}"/>
+    <workbookView xWindow="35340" yWindow="4335" windowWidth="17280" windowHeight="8880" firstSheet="4" activeTab="5" xr2:uid="{D341BFEF-FEF1-4343-8272-FBF06FB03C18}"/>
   </bookViews>
   <sheets>
     <sheet name="PersonalAutoData" sheetId="1" r:id="rId1"/>
     <sheet name="CustomerData" sheetId="4" r:id="rId2"/>
     <sheet name="VehicleData" sheetId="6" r:id="rId3"/>
     <sheet name="EndorsementData" sheetId="7" r:id="rId4"/>
-    <sheet name="Diary" sheetId="10" r:id="rId5"/>
-    <sheet name="CancelationData" sheetId="8" r:id="rId6"/>
+    <sheet name="DiaryData" sheetId="10" r:id="rId5"/>
+    <sheet name="CancellationData" sheetId="8" r:id="rId6"/>
     <sheet name="ReinstatementData" sheetId="9" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191028"/>
@@ -221,9 +221,6 @@
     <t>License_State/Province</t>
   </si>
   <si>
-    <t>1/5/1995</t>
-  </si>
-  <si>
     <t>8/26/1986</t>
   </si>
   <si>
@@ -305,7 +302,10 @@
     <t>test@test.test</t>
   </si>
   <si>
-    <t>test</t>
+    <t>1/5/2003</t>
+  </si>
+  <si>
+    <t>Smoke test</t>
   </si>
 </sst>
 </file>
@@ -826,7 +826,7 @@
         <v>56</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>10</v>
@@ -861,8 +861,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82C167A2-CD5C-4977-B794-BF3104AB0DCB}">
   <dimension ref="A1:L3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L3" sqref="L3"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -939,7 +939,7 @@
         <v>53</v>
       </c>
       <c r="G2" s="10" t="s">
-        <v>59</v>
+        <v>86</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>22</v>
@@ -977,7 +977,7 @@
         <v>53</v>
       </c>
       <c r="G3" s="10" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H3" s="1" t="s">
         <v>12</v>
@@ -1047,7 +1047,7 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>16</v>
@@ -1056,7 +1056,7 @@
         <v>37</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>17</v>
@@ -1070,7 +1070,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>23</v>
@@ -1115,49 +1115,49 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="12" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C1" s="12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D1" s="12" t="s">
         <v>55</v>
       </c>
       <c r="E1" s="12" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>69</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>70</v>
       </c>
       <c r="D2" s="1"/>
       <c r="E2" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>69</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>70</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
   </sheetData>
@@ -1169,8 +1169,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{577AC688-EAD9-49D4-9F20-14C709916D15}">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1182,30 +1182,30 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="B1" s="12" t="s">
         <v>81</v>
-      </c>
-      <c r="B1" s="12" t="s">
-        <v>82</v>
       </c>
       <c r="C1" s="12" t="s">
         <v>30</v>
       </c>
       <c r="D1" s="12" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E1" s="12" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>84</v>
-      </c>
       <c r="C2" s="13" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>87</v>
@@ -1226,13 +1226,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D49D3F3-CDFD-45AB-BBBE-4F6B62388EC6}">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:E1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.33203125" customWidth="1"/>
+    <col min="1" max="1" width="20.109375" customWidth="1"/>
     <col min="2" max="2" width="13.33203125" customWidth="1"/>
     <col min="3" max="3" width="11.33203125" customWidth="1"/>
     <col min="4" max="4" width="8.77734375" customWidth="1"/>
@@ -1241,38 +1241,39 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="12" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B1" s="12" t="s">
         <v>55</v>
       </c>
       <c r="C1" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="D1" s="12" t="s">
         <v>65</v>
       </c>
-      <c r="D1" s="12" t="s">
-        <v>66</v>
-      </c>
       <c r="E1" s="12" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>75</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>76</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1294,34 +1295,34 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="12" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B1" s="12" t="s">
         <v>55</v>
       </c>
       <c r="C1" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="D1" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="E1" s="12" t="s">
         <v>65</v>
-      </c>
-      <c r="D1" s="12" t="s">
-        <v>77</v>
-      </c>
-      <c r="E1" s="12" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D2" s="11" t="s">
         <v>11</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added effective dates fora ll transactions to test data
</commit_message>
<xml_diff>
--- a/CucumberTest/src/TestData/TestData.xlsx
+++ b/CucumberTest/src/TestData/TestData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NastasjaDamjanac\Desktop\SmokeSandbox\Sandbox-Automation-Smoke-Test\CucumberTest\src\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adragutinovic\Desktop\Projekti\Sandbox Smoke\Sandbox-Automation-Smoke-Test\Sandbox-Automation-Smoke-Test\CucumberTest\src\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F325126D-7237-44F8-B184-029DA25F4740}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F972943-63DE-42AE-8958-A3890B18BCCF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="35340" yWindow="4335" windowWidth="17280" windowHeight="8880" firstSheet="4" activeTab="5" xr2:uid="{D341BFEF-FEF1-4343-8272-FBF06FB03C18}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="1" activeTab="3" xr2:uid="{D341BFEF-FEF1-4343-8272-FBF06FB03C18}"/>
   </bookViews>
   <sheets>
     <sheet name="PersonalAutoData" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="92">
   <si>
     <t>Program</t>
   </si>
@@ -306,6 +306,18 @@
   </si>
   <si>
     <t>Smoke test</t>
+  </si>
+  <si>
+    <t>12/01/2024</t>
+  </si>
+  <si>
+    <t>12/02/2024</t>
+  </si>
+  <si>
+    <t>19/02/2024</t>
+  </si>
+  <si>
+    <t>27/01/2024</t>
   </si>
 </sst>
 </file>
@@ -1100,8 +1112,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19DA6AE0-FD1B-43DF-B1FC-EADB519F14FB}">
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1140,7 +1152,9 @@
       <c r="C2" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="D2" s="1"/>
+      <c r="D2" s="3" t="s">
+        <v>88</v>
+      </c>
       <c r="E2" s="1" t="s">
         <v>70</v>
       </c>
@@ -1155,7 +1169,9 @@
       <c r="C3" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="D3" s="1"/>
+      <c r="D3" s="3" t="s">
+        <v>91</v>
+      </c>
       <c r="E3" s="1" t="s">
         <v>79</v>
       </c>
@@ -1226,8 +1242,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D49D3F3-CDFD-45AB-BBBE-4F6B62388EC6}">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1260,7 +1276,9 @@
       <c r="A2" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="B2" s="1"/>
+      <c r="B2" s="3" t="s">
+        <v>89</v>
+      </c>
       <c r="C2" s="1" t="s">
         <v>73</v>
       </c>
@@ -1282,7 +1300,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1314,7 +1332,9 @@
       <c r="A2" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="B2" s="1"/>
+      <c r="B2" s="3" t="s">
+        <v>90</v>
+      </c>
       <c r="C2" s="1" t="s">
         <v>77</v>
       </c>

</xml_diff>

<commit_message>
Added steps in feature file and basic asserts
</commit_message>
<xml_diff>
--- a/CucumberTest/src/TestData/TestData.xlsx
+++ b/CucumberTest/src/TestData/TestData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adragutinovic\Desktop\Projekti\Sandbox Smoke\Sandbox-Automation-Smoke-Test\Sandbox-Automation-Smoke-Test\CucumberTest\src\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NastasjaDamjanac\Desktop\SmokeSandbox\Sandbox-Automation-Smoke-Test\CucumberTest\src\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F972943-63DE-42AE-8958-A3890B18BCCF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43F4368F-FB3D-48BC-8A0C-322AA51D8185}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="1" activeTab="3" xr2:uid="{D341BFEF-FEF1-4343-8272-FBF06FB03C18}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{D341BFEF-FEF1-4343-8272-FBF06FB03C18}"/>
   </bookViews>
   <sheets>
     <sheet name="PersonalAutoData" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="92">
   <si>
     <t>Program</t>
   </si>
@@ -871,10 +871,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82C167A2-CD5C-4977-B794-BF3104AB0DCB}">
-  <dimension ref="A1:L3"/>
+  <dimension ref="A1:M3"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M1" sqref="M1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -891,9 +891,10 @@
     <col min="10" max="10" width="14.44140625" customWidth="1"/>
     <col min="11" max="11" width="19.33203125" customWidth="1"/>
     <col min="12" max="12" width="35.6640625" customWidth="1"/>
+    <col min="13" max="13" width="12.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
         <v>32</v>
       </c>
@@ -930,8 +931,11 @@
       <c r="L1" s="6" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="M1" s="6" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>29</v>
       </c>
@@ -968,8 +972,11 @@
       <c r="L2" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="M2" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>24</v>
       </c>
@@ -1005,6 +1012,9 @@
       </c>
       <c r="L3" s="1" t="s">
         <v>11</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>52</v>
       </c>
     </row>
   </sheetData>
@@ -1022,7 +1032,7 @@
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:C3"/>
+      <selection activeCell="G3" sqref="G1:G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1112,8 +1122,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19DA6AE0-FD1B-43DF-B1FC-EADB519F14FB}">
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1300,7 +1310,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1347,5 +1357,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>